<commit_message>
again up on the LB
</commit_message>
<xml_diff>
--- a/output/experiments.xlsx
+++ b/output/experiments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>Train</t>
   </si>
@@ -140,6 +140,84 @@
   </si>
   <si>
     <t>stacking model train 0.0880, test 0.1066</t>
+  </si>
+  <si>
+    <t>train 0.09118, test 0.10955</t>
+  </si>
+  <si>
+    <t>categorifying certain columns doesnt help</t>
+  </si>
+  <si>
+    <t>train 0.09432, test 0.11155</t>
+  </si>
+  <si>
+    <t>box cox of skewed features</t>
+  </si>
+  <si>
+    <t>train 0.09603, test 0.11480</t>
+  </si>
+  <si>
+    <t>log of skewed features</t>
+  </si>
+  <si>
+    <t>nothing done with skewness</t>
+  </si>
+  <si>
+    <t>train 0.09148, test 0.11241</t>
+  </si>
+  <si>
+    <t>RobustScaler</t>
+  </si>
+  <si>
+    <t>NEW lasso baseline</t>
+  </si>
+  <si>
+    <t>train 0.09576, test 0.10799</t>
+  </si>
+  <si>
+    <t>train 0.09564, test 0.10790</t>
+  </si>
+  <si>
+    <t>added  some HASx features</t>
+  </si>
+  <si>
+    <t>train 0.09567, test 0.10789</t>
+  </si>
+  <si>
+    <t>remove id</t>
+  </si>
+  <si>
+    <t>train 0.09482, test 0.10760</t>
+  </si>
+  <si>
+    <t>adding log and squared features</t>
+  </si>
+  <si>
+    <t>train 0.09483, test 0.10757</t>
+  </si>
+  <si>
+    <t>only  log features</t>
+  </si>
+  <si>
+    <t>train 0.09459, test 0.10789</t>
+  </si>
+  <si>
+    <t>ex squeard</t>
+  </si>
+  <si>
+    <t>train 0.11129, test 0.12011</t>
+  </si>
+  <si>
+    <t>ex third</t>
+  </si>
+  <si>
+    <t>train 0.09463, test 0.10778</t>
+  </si>
+  <si>
+    <t>ex second</t>
+  </si>
+  <si>
+    <t>stacking model train 0.0831, test 0.1062</t>
   </si>
 </sst>
 </file>
@@ -149,10 +227,10 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +252,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="var(--vscode-editor-font-family"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -187,16 +271,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,8 +301,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,24 +333,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,40 +362,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,187 +410,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -517,6 +601,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -539,40 +662,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,17 +682,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -622,7 +706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -640,134 +724,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -778,6 +862,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1146,10 +1233,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1369,8 +1456,119 @@
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>